<commit_message>
Population except age zero
</commit_message>
<xml_diff>
--- a/serra_da_estrela_cheese.xlsx
+++ b/serra_da_estrela_cheese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulisboa-my.sharepoint.com/personal/costaraquel_office365_ulisboa_pt/Documents/Faculdade/6 ano/Classic QMRA/intern_dtu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{026A19C0-ACA6-49AD-AF13-DD7F088AD614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4B00A089-36DD-4F43-896C-0C5DD808F631}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="8_{026A19C0-ACA6-49AD-AF13-DD7F088AD614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97D39DFB-D2B9-4DA1-8D34-2DF45E6DE467}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D953F70C-7EF8-4AB4-B49F-B373F82087BA}"/>
   </bookViews>
@@ -704,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F2D110-5AD7-4F9E-8B3A-649A1D362D9C}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,11 +764,11 @@
         <v>3</v>
       </c>
       <c r="G2" s="20">
-        <v>219323</v>
+        <v>176893</v>
       </c>
       <c r="H2" s="20">
         <f>E2*F2*G2</f>
-        <v>7459965.9863945572</v>
+        <v>6016768.7074829927</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -792,11 +792,11 @@
         <v>3</v>
       </c>
       <c r="G3" s="20">
-        <v>229680</v>
+        <v>185123</v>
       </c>
       <c r="H3" s="20">
         <f t="shared" ref="H3:H15" si="1">E3*F3*G3</f>
-        <v>7812244.897959183</v>
+        <v>6296700.6802721079</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>